<commit_message>
updates and add file
</commit_message>
<xml_diff>
--- a/docs/assets/files/verwerking_mailing1_vansteendam_jarne.xlsx
+++ b/docs/assets/files/verwerking_mailing1_vansteendam_jarne.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Jarne\artevelde\pgm-code\19-20\busicom\mailing\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jarne\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69069BBC-4580-491E-B23A-425B23A35DBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3602CCCC-A23E-4FC6-A0DC-769DF0E67D70}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{74FC18E7-9878-4CF6-A1C3-B1A74B536DAF}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
-  <si>
-    <t>Verwerking Mailing 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>Percentage geopend</t>
   </si>
@@ -43,9 +40,6 @@
   </si>
   <si>
     <t>Aantal geopend</t>
-  </si>
-  <si>
-    <t>Mail geklikt</t>
   </si>
   <si>
     <t>Aantal geklikt</t>
@@ -67,9 +61,6 @@
   </si>
   <si>
     <t>Jaimy Van Gyseghem</t>
-  </si>
-  <si>
-    <t>Selina Topke</t>
   </si>
   <si>
     <t>Lennert De Ryck</t>
@@ -136,6 +127,18 @@
   </si>
   <si>
     <t>Percentage ingevuld</t>
+  </si>
+  <si>
+    <t>Aantal invullers</t>
+  </si>
+  <si>
+    <t>Verwerking mailing 1</t>
+  </si>
+  <si>
+    <t>Selina Töpke</t>
+  </si>
+  <si>
+    <t>Mail geklikt (uniek aantal)</t>
   </si>
 </sst>
 </file>
@@ -244,13 +247,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3500,10 +3503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FD1F37-BE33-45AD-A674-0B8B8C4AC2DA}">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3517,78 +3520,80 @@
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
+    <row r="1" spans="1:18" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
     </row>
-    <row r="3" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+    <row r="3" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2">
         <v>35</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="6"/>
+      <c r="G3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="5"/>
       <c r="I3" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="J3" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="G5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="7"/>
+      <c r="G5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>E3</f>
         <v>35</v>
@@ -3601,113 +3606,113 @@
         <v>0.51428571428571423</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6"/>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>7</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="7"/>
+      <c r="G13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="G15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
         <v>3</v>
       </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -3726,7 +3731,7 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="G17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -3734,19 +3739,19 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H18">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="7"/>
+      <c r="A19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="6"/>
       <c r="G19" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H19">
         <v>6</v>
@@ -3754,47 +3759,47 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H21" s="7"/>
+      <c r="G21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -3802,7 +3807,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -3810,12 +3815,12 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="G25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -3823,16 +3828,16 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H26">
         <v>7</v>
@@ -3852,7 +3857,7 @@
         <v>0.875</v>
       </c>
       <c r="G27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H27">
         <v>7</v>
@@ -3860,12 +3865,12 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G29" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G30" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H30" s="4"/>
     </row>
@@ -3875,7 +3880,7 @@
     </row>
     <row r="33" spans="7:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G33" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H33" s="4"/>
     </row>
@@ -3884,7 +3889,6 @@
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="G30:H31"/>
     <mergeCell ref="G33:H33"/>
-    <mergeCell ref="A1:P1"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="G5:H5"/>
@@ -3894,6 +3898,7 @@
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:R1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>